<commit_message>
Deploying to gh-pages from  @ 0c421bb697e4bbf2fb4ad27fd5b7d3d06198eaab 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2023_4-1-2.xlsx
+++ b/assets/excel/2023_4-1-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15_Uebergreifende_Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C00A3D3-9BD9-45E3-BD85-D95337F95DD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08B8267-5BAA-4A62-8753-F31270D84C53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{EAD2624E-AA52-4F6A-A4A2-2F5595CC88FF}"/>
   </bookViews>
@@ -123,12 +123,6 @@
     <t>1) Schulischer Teil</t>
   </si>
   <si>
-    <t>2) Abschluss Förderschule Lernen und Geistige Entwicklung</t>
-  </si>
-  <si>
-    <t>3) Die überdurchschnittlichen Veränderungen bei den Absolventinnen und Absolventen mit allgemeiner Hochschulreife sind dadurch bestimmt, dass es im Schuljahr 2019/2020 wegen der Rückkehr zum 9-jährigen Bildungsgang an Gymnasien, keinen vollständigen Abiturjahrgang gab.</t>
-  </si>
-  <si>
     <t>Quelle: Schulstatistik</t>
   </si>
   <si>
@@ -142,6 +136,12 @@
   </si>
   <si>
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
+  <si>
+    <t>Hinweis: Die überdurchschnittlichen Veränderungen bei den Absolventinnen und Absolventen mit allgemeiner Hochschulreife sind dadurch bestimmt, dass es im Schuljahr 2019/2020 wegen der Rückkehr zum 9-jährigen Bildungsgang an Gymnasien, keinen vollständigen Abiturjahrgang gab.</t>
+  </si>
+  <si>
+    <t>2) Abschluss Förderschule Lernen und Abgang Förderschule Geistige Entwicklung</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -406,37 +406,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -465,34 +435,16 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -503,18 +455,12 @@
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -524,43 +470,13 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -597,6 +513,81 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -914,7 +905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6D33F1A-F31E-4532-9F06-D1067EBF3F01}">
   <dimension ref="B1:O119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -963,2178 +954,2178 @@
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="54" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="55"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="15"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="16" t="s">
+      <c r="B9" s="50"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="L9" s="18" t="s">
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="L9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="M9" s="18" t="s">
+      <c r="M9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="N9" s="18" t="s">
+      <c r="N9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="16">
         <v>2022</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="17">
         <v>24810</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="17">
         <v>23983</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="17">
         <v>827</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="16">
         <v>2022</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="17">
         <v>2289</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="17">
         <v>2102</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="17">
         <v>187</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="16">
         <v>2022</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="17">
         <v>33410</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="17">
         <v>30088</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="17">
         <v>3322</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="16">
         <v>2022</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="17">
         <v>10646</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="17">
         <v>8761</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="17">
         <v>1885</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="16">
         <v>2022</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="17">
         <v>2228</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="17">
         <v>1821</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="17">
         <v>407</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="16">
         <v>2022</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="17">
         <v>2858</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="17">
         <v>1818</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="17">
         <v>1040</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-    </row>
-    <row r="17" spans="2:15" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="24" t="s">
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+    </row>
+    <row r="17" spans="2:15" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="58">
         <v>2022</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D17" s="59">
         <v>76241</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="59">
         <v>68573</v>
       </c>
-      <c r="F17" s="29">
+      <c r="F17" s="59">
         <v>7668</v>
       </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-    </row>
-    <row r="18" spans="2:15" s="14" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="22" t="s">
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+    </row>
+    <row r="18" spans="2:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="16">
         <v>2021</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="17">
         <v>25484</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="17">
         <v>24894</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="17">
         <v>590</v>
       </c>
     </row>
-    <row r="19" spans="2:15" s="14" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="22" t="s">
+    <row r="19" spans="2:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="16">
         <v>2021</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="17">
         <v>1997</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="17">
         <v>1866</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="17">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:15" s="14" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="22" t="s">
+    <row r="20" spans="2:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="16">
         <v>2021</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="17">
         <v>33930</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="17">
         <v>30950</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="17">
         <v>2980</v>
       </c>
     </row>
-    <row r="21" spans="2:15" s="14" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="22" t="s">
+    <row r="21" spans="2:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="16">
         <v>2021</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="17">
         <v>10318</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="17">
         <v>8716</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="17">
         <v>1602</v>
       </c>
     </row>
-    <row r="22" spans="2:15" s="14" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+    <row r="22" spans="2:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="16">
         <v>2021</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="17">
         <v>2188</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="17">
         <v>1828</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="17">
         <v>360</v>
       </c>
     </row>
-    <row r="23" spans="2:15" s="14" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22" t="s">
+    <row r="23" spans="2:15" s="7" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="16">
         <v>2021</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="17">
         <v>2402</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E23" s="17">
         <v>1548</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="17">
         <v>854</v>
       </c>
     </row>
-    <row r="24" spans="2:15" s="25" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="24" t="s">
+    <row r="24" spans="2:15" s="15" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="58">
         <v>2021</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="59">
         <v>76319</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="59">
         <v>69802</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="59">
         <v>6517</v>
       </c>
     </row>
     <row r="25" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="16">
         <v>2020</v>
       </c>
-      <c r="D25" s="27">
+      <c r="D25" s="17">
         <v>5198</v>
       </c>
-      <c r="E25" s="27">
+      <c r="E25" s="17">
         <v>5039</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="17">
         <v>159</v>
       </c>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="14"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="16">
         <v>2020</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="17">
         <v>1693</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E26" s="17">
         <v>1592</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="17">
         <v>101</v>
       </c>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="16">
         <v>2020</v>
       </c>
-      <c r="D27" s="27">
+      <c r="D27" s="17">
         <v>35249</v>
       </c>
-      <c r="E27" s="27">
+      <c r="E27" s="17">
         <v>32466</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="17">
         <v>2783</v>
       </c>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
     </row>
     <row r="28" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="16">
         <v>2020</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="17">
         <v>10566</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="17">
         <v>8882</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="17">
         <v>1684</v>
       </c>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
-      <c r="L28" s="14"/>
-      <c r="M28" s="14"/>
-      <c r="N28" s="14"/>
-      <c r="O28" s="14"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="16">
         <v>2020</v>
       </c>
-      <c r="D29" s="27">
+      <c r="D29" s="17">
         <v>2157</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="17">
         <v>1853</v>
       </c>
-      <c r="F29" s="27">
+      <c r="F29" s="17">
         <v>304</v>
       </c>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="16">
         <v>2020</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="17">
         <v>2455</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="17">
         <v>1543</v>
       </c>
-      <c r="F30" s="27">
+      <c r="F30" s="17">
         <v>912</v>
       </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
-      <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-    </row>
-    <row r="31" spans="2:15" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="24" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+    </row>
+    <row r="31" spans="2:15" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="58">
         <v>2020</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="59">
         <v>57318</v>
       </c>
-      <c r="E31" s="29">
+      <c r="E31" s="59">
         <v>51375</v>
       </c>
-      <c r="F31" s="29">
+      <c r="F31" s="59">
         <v>5943</v>
       </c>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="15"/>
+      <c r="O31" s="15"/>
     </row>
     <row r="32" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="16">
         <v>2019</v>
       </c>
-      <c r="D32" s="30">
+      <c r="D32" s="18">
         <v>27080</v>
       </c>
-      <c r="E32" s="30">
+      <c r="E32" s="18">
         <v>26426</v>
       </c>
-      <c r="F32" s="30">
+      <c r="F32" s="18">
         <v>654</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
-      <c r="L32" s="14"/>
-      <c r="M32" s="14"/>
-      <c r="N32" s="14"/>
-      <c r="O32" s="14"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="16">
         <v>2019</v>
       </c>
-      <c r="D33" s="30">
+      <c r="D33" s="18">
         <v>2350</v>
       </c>
-      <c r="E33" s="30">
+      <c r="E33" s="18">
         <v>2205</v>
       </c>
-      <c r="F33" s="30">
+      <c r="F33" s="18">
         <v>145</v>
       </c>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
-      <c r="L33" s="14"/>
-      <c r="M33" s="14"/>
-      <c r="N33" s="14"/>
-      <c r="O33" s="14"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
     <row r="34" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="16">
         <v>2019</v>
       </c>
-      <c r="D34" s="30">
+      <c r="D34" s="18">
         <v>34113</v>
       </c>
-      <c r="E34" s="30">
+      <c r="E34" s="18">
         <v>31449</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="18">
         <v>2664</v>
       </c>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="L34" s="14"/>
-      <c r="M34" s="14"/>
-      <c r="N34" s="14"/>
-      <c r="O34" s="14"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
     </row>
     <row r="35" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="16">
         <v>2019</v>
       </c>
-      <c r="D35" s="30">
+      <c r="D35" s="18">
         <v>11205</v>
       </c>
-      <c r="E35" s="30">
+      <c r="E35" s="18">
         <v>9629</v>
       </c>
-      <c r="F35" s="30">
+      <c r="F35" s="18">
         <v>1576</v>
       </c>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
-      <c r="N35" s="14"/>
-      <c r="O35" s="14"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
     </row>
     <row r="36" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="16">
         <v>2019</v>
       </c>
-      <c r="D36" s="30">
+      <c r="D36" s="18">
         <v>2067</v>
       </c>
-      <c r="E36" s="30">
+      <c r="E36" s="18">
         <v>1832</v>
       </c>
-      <c r="F36" s="30">
+      <c r="F36" s="18">
         <v>235</v>
       </c>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="L36" s="14"/>
-      <c r="M36" s="14"/>
-      <c r="N36" s="14"/>
-      <c r="O36" s="14"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="16">
         <v>2019</v>
       </c>
-      <c r="D37" s="30">
+      <c r="D37" s="18">
         <v>3357</v>
       </c>
-      <c r="E37" s="30">
+      <c r="E37" s="18">
         <v>2076</v>
       </c>
-      <c r="F37" s="30">
+      <c r="F37" s="18">
         <v>1281</v>
       </c>
-      <c r="G37" s="31"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-    </row>
-    <row r="38" spans="2:15" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="24" t="s">
+      <c r="G37" s="19"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
+    </row>
+    <row r="38" spans="2:15" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C38" s="24">
+      <c r="C38" s="60">
         <v>2019</v>
       </c>
-      <c r="D38" s="32">
+      <c r="D38" s="61">
         <v>80172</v>
       </c>
-      <c r="E38" s="32">
+      <c r="E38" s="61">
         <v>73617</v>
       </c>
-      <c r="F38" s="32">
+      <c r="F38" s="61">
         <v>6555</v>
       </c>
-      <c r="G38" s="33"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-      <c r="O38" s="25"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="15"/>
     </row>
     <row r="39" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="21" t="s">
+      <c r="B39" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="16">
         <v>2018</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="62">
         <v>26523</v>
       </c>
-      <c r="E39" s="35">
+      <c r="E39" s="18">
         <v>25872</v>
       </c>
-      <c r="F39" s="35">
+      <c r="F39" s="18">
         <v>651</v>
       </c>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
     </row>
     <row r="40" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="16">
         <v>2018</v>
       </c>
-      <c r="D40" s="34">
+      <c r="D40" s="62">
         <v>2341</v>
       </c>
-      <c r="E40" s="35">
+      <c r="E40" s="18">
         <v>2216</v>
       </c>
-      <c r="F40" s="35">
+      <c r="F40" s="18">
         <v>125</v>
       </c>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
-      <c r="L40" s="14"/>
-      <c r="M40" s="14"/>
-      <c r="N40" s="14"/>
-      <c r="O40" s="14"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
     </row>
     <row r="41" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="16">
         <v>2018</v>
       </c>
-      <c r="D41" s="34">
+      <c r="D41" s="62">
         <v>35591</v>
       </c>
-      <c r="E41" s="35">
+      <c r="E41" s="18">
         <v>33213</v>
       </c>
-      <c r="F41" s="35">
+      <c r="F41" s="18">
         <v>2378</v>
       </c>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
     </row>
     <row r="42" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C42" s="26">
+      <c r="C42" s="16">
         <v>2018</v>
       </c>
-      <c r="D42" s="34">
+      <c r="D42" s="62">
         <v>11516</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="62">
         <v>9853</v>
       </c>
-      <c r="F42" s="34">
+      <c r="F42" s="62">
         <v>1663</v>
       </c>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
     </row>
     <row r="43" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="26">
+      <c r="C43" s="16">
         <v>2018</v>
       </c>
-      <c r="D43" s="34">
+      <c r="D43" s="62">
         <v>1963</v>
       </c>
-      <c r="E43" s="35">
+      <c r="E43" s="18">
         <v>1751</v>
       </c>
-      <c r="F43" s="35">
+      <c r="F43" s="18">
         <v>212</v>
       </c>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
     </row>
     <row r="44" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="26">
+      <c r="C44" s="16">
         <v>2018</v>
       </c>
-      <c r="D44" s="34">
+      <c r="D44" s="62">
         <v>3130</v>
       </c>
-      <c r="E44" s="35">
+      <c r="E44" s="18">
         <v>1915</v>
       </c>
-      <c r="F44" s="35">
+      <c r="F44" s="18">
         <v>1215</v>
       </c>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
-      <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-    </row>
-    <row r="45" spans="2:15" s="36" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="24" t="s">
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+    </row>
+    <row r="45" spans="2:15" s="21" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C45" s="37">
+      <c r="C45" s="63">
         <v>2018</v>
       </c>
-      <c r="D45" s="38">
+      <c r="D45" s="22">
         <v>81064</v>
       </c>
-      <c r="E45" s="38">
+      <c r="E45" s="22">
         <v>74820</v>
       </c>
-      <c r="F45" s="38">
+      <c r="F45" s="22">
         <v>6244</v>
       </c>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="39"/>
+      <c r="G45" s="23"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
     </row>
     <row r="46" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="21" t="s">
+      <c r="B46" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C46" s="40">
+      <c r="C46" s="24">
         <v>2017</v>
       </c>
-      <c r="D46" s="38">
+      <c r="D46" s="22">
         <v>26734</v>
       </c>
-      <c r="E46" s="38">
+      <c r="E46" s="22">
         <v>26092</v>
       </c>
-      <c r="F46" s="38">
+      <c r="F46" s="22">
         <v>642</v>
       </c>
-      <c r="G46" s="41"/>
-      <c r="H46" s="41"/>
-      <c r="I46" s="41"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41"/>
-      <c r="O46" s="41"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="25"/>
+      <c r="O46" s="25"/>
     </row>
     <row r="47" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="21" t="s">
+      <c r="B47" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="40">
+      <c r="C47" s="24">
         <v>2017</v>
       </c>
-      <c r="D47" s="38">
+      <c r="D47" s="22">
         <v>2183</v>
       </c>
-      <c r="E47" s="38">
+      <c r="E47" s="22">
         <v>2019</v>
       </c>
-      <c r="F47" s="38">
+      <c r="F47" s="22">
         <v>164</v>
       </c>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="41"/>
-      <c r="M47" s="41"/>
-      <c r="N47" s="41"/>
-      <c r="O47" s="41"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="25"/>
+      <c r="O47" s="25"/>
     </row>
     <row r="48" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="40">
+      <c r="C48" s="24">
         <v>2017</v>
       </c>
-      <c r="D48" s="38">
+      <c r="D48" s="22">
         <v>37000</v>
       </c>
-      <c r="E48" s="38">
+      <c r="E48" s="22">
         <v>34782</v>
       </c>
-      <c r="F48" s="38">
+      <c r="F48" s="22">
         <v>2218</v>
       </c>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="41"/>
-      <c r="O48" s="41"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="25"/>
+      <c r="O48" s="25"/>
     </row>
     <row r="49" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C49" s="40">
+      <c r="C49" s="24">
         <v>2017</v>
       </c>
-      <c r="D49" s="38">
+      <c r="D49" s="22">
         <v>11686</v>
       </c>
-      <c r="E49" s="38">
+      <c r="E49" s="22">
         <v>10305</v>
       </c>
-      <c r="F49" s="38">
+      <c r="F49" s="22">
         <v>1381</v>
       </c>
-      <c r="G49" s="41"/>
-      <c r="H49" s="41"/>
-      <c r="I49" s="41"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="41"/>
-      <c r="M49" s="41"/>
-      <c r="N49" s="41"/>
-      <c r="O49" s="41"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="25"/>
+      <c r="O49" s="25"/>
     </row>
     <row r="50" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="40">
+      <c r="C50" s="24">
         <v>2017</v>
       </c>
-      <c r="D50" s="38">
+      <c r="D50" s="22">
         <v>1692</v>
       </c>
-      <c r="E50" s="38">
+      <c r="E50" s="22">
         <v>1507</v>
       </c>
-      <c r="F50" s="38">
+      <c r="F50" s="22">
         <v>185</v>
       </c>
-      <c r="G50" s="41"/>
-      <c r="H50" s="41"/>
-      <c r="I50" s="41"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
-      <c r="O50" s="41"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
     </row>
     <row r="51" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="22" t="s">
+      <c r="B51" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="40">
+      <c r="C51" s="24">
         <v>2017</v>
       </c>
-      <c r="D51" s="42">
+      <c r="D51" s="64">
         <v>3138</v>
       </c>
-      <c r="E51" s="42">
+      <c r="E51" s="64">
         <v>2013</v>
       </c>
-      <c r="F51" s="42">
+      <c r="F51" s="64">
         <v>1125</v>
       </c>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="41"/>
-      <c r="O51" s="41"/>
-    </row>
-    <row r="52" spans="2:15" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="24" t="s">
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+      <c r="O51" s="25"/>
+    </row>
+    <row r="52" spans="2:15" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="37">
+      <c r="C52" s="63">
         <v>2017</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="64">
         <v>82433</v>
       </c>
-      <c r="E52" s="42">
+      <c r="E52" s="64">
         <v>76718</v>
       </c>
-      <c r="F52" s="42">
+      <c r="F52" s="64">
         <v>5715</v>
       </c>
-      <c r="G52" s="43"/>
-      <c r="H52" s="43"/>
-      <c r="I52" s="43"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="43"/>
-      <c r="N52" s="43"/>
-      <c r="O52" s="43"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="26"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="26"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
     </row>
     <row r="53" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C53" s="40">
+      <c r="C53" s="24">
         <v>2016</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D53" s="22">
         <v>27554</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E53" s="22">
         <v>26873</v>
       </c>
-      <c r="F53" s="38">
+      <c r="F53" s="22">
         <v>681</v>
       </c>
-      <c r="G53" s="41"/>
-      <c r="H53" s="41"/>
-      <c r="I53" s="41"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
-      <c r="L53" s="41"/>
-      <c r="M53" s="41"/>
-      <c r="N53" s="41"/>
-      <c r="O53" s="41"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
     </row>
     <row r="54" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C54" s="40">
+      <c r="C54" s="24">
         <v>2016</v>
       </c>
-      <c r="D54" s="38">
+      <c r="D54" s="22">
         <v>1918</v>
       </c>
-      <c r="E54" s="38">
+      <c r="E54" s="22">
         <v>1802</v>
       </c>
-      <c r="F54" s="38">
+      <c r="F54" s="22">
         <v>116</v>
       </c>
-      <c r="G54" s="44"/>
-      <c r="H54" s="44"/>
-      <c r="I54" s="44"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="44"/>
-      <c r="M54" s="44"/>
-      <c r="N54" s="44"/>
-      <c r="O54" s="44"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="27"/>
+      <c r="N54" s="27"/>
+      <c r="O54" s="27"/>
     </row>
     <row r="55" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="22" t="s">
+      <c r="B55" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="40">
+      <c r="C55" s="24">
         <v>2016</v>
       </c>
-      <c r="D55" s="38">
+      <c r="D55" s="22">
         <v>39059</v>
       </c>
-      <c r="E55" s="38">
+      <c r="E55" s="22">
         <v>36674</v>
       </c>
-      <c r="F55" s="38">
+      <c r="F55" s="22">
         <v>2385</v>
       </c>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
-      <c r="L55" s="14"/>
-      <c r="M55" s="14"/>
-      <c r="N55" s="14"/>
-      <c r="O55" s="14"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
     </row>
     <row r="56" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="22" t="s">
+      <c r="B56" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="40">
+      <c r="C56" s="24">
         <v>2016</v>
       </c>
-      <c r="D56" s="38">
+      <c r="D56" s="22">
         <v>11333</v>
       </c>
-      <c r="E56" s="38">
+      <c r="E56" s="22">
         <v>10096</v>
       </c>
-      <c r="F56" s="38">
+      <c r="F56" s="22">
         <v>1237</v>
       </c>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-      <c r="L56" s="14"/>
-      <c r="M56" s="14"/>
-      <c r="N56" s="14"/>
-      <c r="O56" s="14"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
     </row>
     <row r="57" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="22" t="s">
+      <c r="B57" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="40">
+      <c r="C57" s="24">
         <v>2016</v>
       </c>
-      <c r="D57" s="38">
+      <c r="D57" s="22">
         <v>1780</v>
       </c>
-      <c r="E57" s="38">
+      <c r="E57" s="22">
         <v>1582</v>
       </c>
-      <c r="F57" s="38">
+      <c r="F57" s="22">
         <v>198</v>
       </c>
     </row>
     <row r="58" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="22" t="s">
+      <c r="B58" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="40">
+      <c r="C58" s="24">
         <v>2016</v>
       </c>
-      <c r="D58" s="38">
+      <c r="D58" s="22">
         <v>2511</v>
       </c>
-      <c r="E58" s="38">
+      <c r="E58" s="22">
         <v>1849</v>
       </c>
-      <c r="F58" s="38">
+      <c r="F58" s="22">
         <v>662</v>
       </c>
     </row>
-    <row r="59" spans="2:15" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="24" t="s">
+    <row r="59" spans="2:15" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="37">
+      <c r="C59" s="63">
         <v>2016</v>
       </c>
-      <c r="D59" s="42">
+      <c r="D59" s="64">
         <v>84155</v>
       </c>
-      <c r="E59" s="42">
+      <c r="E59" s="64">
         <v>78876</v>
       </c>
-      <c r="F59" s="42">
+      <c r="F59" s="64">
         <v>5279</v>
       </c>
     </row>
     <row r="60" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="21" t="s">
+      <c r="B60" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="40">
+      <c r="C60" s="24">
         <v>2015</v>
       </c>
-      <c r="D60" s="38">
+      <c r="D60" s="22">
         <v>27892</v>
       </c>
-      <c r="E60" s="38">
+      <c r="E60" s="22">
         <v>27241</v>
       </c>
-      <c r="F60" s="38">
+      <c r="F60" s="22">
         <v>651</v>
       </c>
     </row>
     <row r="61" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C61" s="40">
+      <c r="C61" s="24">
         <v>2015</v>
       </c>
-      <c r="D61" s="38">
+      <c r="D61" s="22">
         <v>1797</v>
       </c>
-      <c r="E61" s="38">
+      <c r="E61" s="22">
         <v>1663</v>
       </c>
-      <c r="F61" s="38">
+      <c r="F61" s="22">
         <v>134</v>
       </c>
     </row>
     <row r="62" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="22" t="s">
+      <c r="B62" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="40">
+      <c r="C62" s="24">
         <v>2015</v>
       </c>
-      <c r="D62" s="38">
+      <c r="D62" s="22">
         <v>40641</v>
       </c>
-      <c r="E62" s="38">
+      <c r="E62" s="22">
         <v>37907</v>
       </c>
-      <c r="F62" s="38">
+      <c r="F62" s="22">
         <v>2734</v>
       </c>
     </row>
     <row r="63" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="22" t="s">
+      <c r="B63" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="40">
+      <c r="C63" s="24">
         <v>2015</v>
       </c>
-      <c r="D63" s="38">
+      <c r="D63" s="22">
         <v>11120</v>
       </c>
-      <c r="E63" s="38">
+      <c r="E63" s="22">
         <v>9873</v>
       </c>
-      <c r="F63" s="38">
+      <c r="F63" s="22">
         <v>1247</v>
       </c>
     </row>
     <row r="64" spans="2:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="22" t="s">
+      <c r="B64" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C64" s="40">
+      <c r="C64" s="24">
         <v>2015</v>
       </c>
-      <c r="D64" s="38">
+      <c r="D64" s="22">
         <v>2007</v>
       </c>
-      <c r="E64" s="38">
+      <c r="E64" s="22">
         <v>1727</v>
       </c>
-      <c r="F64" s="38">
+      <c r="F64" s="22">
         <v>280</v>
       </c>
     </row>
     <row r="65" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="22" t="s">
+      <c r="B65" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C65" s="40">
+      <c r="C65" s="24">
         <v>2015</v>
       </c>
-      <c r="D65" s="38">
+      <c r="D65" s="22">
         <v>2332</v>
       </c>
-      <c r="E65" s="38">
+      <c r="E65" s="22">
         <v>1809</v>
       </c>
-      <c r="F65" s="38">
+      <c r="F65" s="22">
         <v>523</v>
       </c>
     </row>
-    <row r="66" spans="2:10" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="24" t="s">
+    <row r="66" spans="2:10" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C66" s="37">
+      <c r="C66" s="63">
         <v>2015</v>
       </c>
-      <c r="D66" s="45">
+      <c r="D66" s="65">
         <v>85789</v>
       </c>
-      <c r="E66" s="32">
+      <c r="E66" s="61">
         <v>80220</v>
       </c>
-      <c r="F66" s="45">
+      <c r="F66" s="65">
         <v>5569</v>
       </c>
     </row>
     <row r="67" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="21" t="s">
+      <c r="B67" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="46">
+      <c r="C67" s="28">
         <v>2014</v>
       </c>
-      <c r="D67" s="47">
+      <c r="D67" s="29">
         <v>26724</v>
       </c>
-      <c r="E67" s="47">
+      <c r="E67" s="29">
         <v>26061</v>
       </c>
-      <c r="F67" s="47">
+      <c r="F67" s="29">
         <v>663</v>
       </c>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="48"/>
+      <c r="G67" s="30"/>
+      <c r="H67" s="30"/>
+      <c r="I67" s="30"/>
     </row>
     <row r="68" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="21" t="s">
+      <c r="B68" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C68" s="46">
+      <c r="C68" s="28">
         <v>2014</v>
       </c>
-      <c r="D68" s="47">
+      <c r="D68" s="29">
         <v>1839</v>
       </c>
-      <c r="E68" s="47">
+      <c r="E68" s="29">
         <v>1700</v>
       </c>
-      <c r="F68" s="47">
+      <c r="F68" s="29">
         <v>139</v>
       </c>
     </row>
     <row r="69" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C69" s="46">
+      <c r="C69" s="28">
         <v>2014</v>
       </c>
-      <c r="D69" s="47">
+      <c r="D69" s="29">
         <v>42449</v>
       </c>
-      <c r="E69" s="47">
+      <c r="E69" s="29">
         <v>39729</v>
       </c>
-      <c r="F69" s="47">
+      <c r="F69" s="29">
         <v>2720</v>
       </c>
     </row>
     <row r="70" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="22" t="s">
+      <c r="B70" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="46">
+      <c r="C70" s="28">
         <v>2014</v>
       </c>
-      <c r="D70" s="47">
+      <c r="D70" s="29">
         <v>12027</v>
       </c>
-      <c r="E70" s="47">
+      <c r="E70" s="29">
         <v>10816</v>
       </c>
-      <c r="F70" s="47">
+      <c r="F70" s="29">
         <v>1211</v>
       </c>
     </row>
     <row r="71" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="22" t="s">
+      <c r="B71" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C71" s="46">
+      <c r="C71" s="28">
         <v>2014</v>
       </c>
-      <c r="D71" s="47">
+      <c r="D71" s="29">
         <v>1964</v>
       </c>
-      <c r="E71" s="47">
+      <c r="E71" s="29">
         <v>1743</v>
       </c>
-      <c r="F71" s="47">
+      <c r="F71" s="29">
         <v>221</v>
       </c>
     </row>
     <row r="72" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="22" t="s">
+      <c r="B72" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C72" s="46">
+      <c r="C72" s="28">
         <v>2014</v>
       </c>
-      <c r="D72" s="47">
+      <c r="D72" s="29">
         <v>2281</v>
       </c>
-      <c r="E72" s="47">
+      <c r="E72" s="29">
         <v>1843</v>
       </c>
-      <c r="F72" s="47">
+      <c r="F72" s="29">
         <v>438</v>
       </c>
     </row>
-    <row r="73" spans="2:10" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="24" t="s">
+    <row r="73" spans="2:10" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C73" s="49">
+      <c r="C73" s="36">
         <v>2014</v>
       </c>
-      <c r="D73" s="50">
+      <c r="D73" s="66">
         <v>87284</v>
       </c>
-      <c r="E73" s="50">
+      <c r="E73" s="66">
         <v>81892</v>
       </c>
-      <c r="F73" s="50">
+      <c r="F73" s="66">
         <v>5392</v>
       </c>
     </row>
     <row r="74" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="21" t="s">
+      <c r="B74" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C74" s="51">
+      <c r="C74" s="28">
         <v>2013</v>
       </c>
-      <c r="D74" s="52">
+      <c r="D74" s="67">
         <v>25788</v>
       </c>
-      <c r="E74" s="35">
+      <c r="E74" s="18">
         <v>25264</v>
       </c>
-      <c r="F74" s="52">
+      <c r="F74" s="67">
         <v>524</v>
       </c>
-      <c r="J74" s="53" t="s">
+      <c r="J74" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="75" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C75" s="51">
+      <c r="C75" s="28">
         <v>2013</v>
       </c>
-      <c r="D75" s="52">
+      <c r="D75" s="67">
         <v>1963</v>
       </c>
-      <c r="E75" s="35">
+      <c r="E75" s="18">
         <v>1881</v>
       </c>
-      <c r="F75" s="52">
+      <c r="F75" s="67">
         <v>82</v>
       </c>
     </row>
     <row r="76" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="22" t="s">
+      <c r="B76" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C76" s="51">
+      <c r="C76" s="28">
         <v>2013</v>
       </c>
-      <c r="D76" s="52">
+      <c r="D76" s="67">
         <v>42205</v>
       </c>
-      <c r="E76" s="35">
+      <c r="E76" s="18">
         <v>39852</v>
       </c>
-      <c r="F76" s="52">
+      <c r="F76" s="67">
         <v>2353</v>
       </c>
     </row>
     <row r="77" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="22" t="s">
+      <c r="B77" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C77" s="51">
+      <c r="C77" s="28">
         <v>2013</v>
       </c>
-      <c r="D77" s="52">
+      <c r="D77" s="67">
         <v>12132</v>
       </c>
-      <c r="E77" s="35">
+      <c r="E77" s="18">
         <v>11000</v>
       </c>
-      <c r="F77" s="52">
+      <c r="F77" s="67">
         <v>1132</v>
       </c>
     </row>
     <row r="78" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="22" t="s">
+      <c r="B78" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C78" s="51">
+      <c r="C78" s="28">
         <v>2013</v>
       </c>
-      <c r="D78" s="52">
+      <c r="D78" s="67">
         <v>2002</v>
       </c>
-      <c r="E78" s="35">
+      <c r="E78" s="18">
         <v>1749</v>
       </c>
-      <c r="F78" s="52">
+      <c r="F78" s="67">
         <v>253</v>
       </c>
     </row>
     <row r="79" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="22" t="s">
+      <c r="B79" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="51">
+      <c r="C79" s="28">
         <v>2013</v>
       </c>
-      <c r="D79" s="52">
+      <c r="D79" s="67">
         <v>2370</v>
       </c>
-      <c r="E79" s="35">
+      <c r="E79" s="18">
         <v>1974</v>
       </c>
-      <c r="F79" s="52">
+      <c r="F79" s="67">
         <v>396</v>
       </c>
     </row>
-    <row r="80" spans="2:10" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="24" t="s">
+    <row r="80" spans="2:10" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C80" s="49">
+      <c r="C80" s="36">
         <v>2013</v>
       </c>
-      <c r="D80" s="54">
+      <c r="D80" s="68">
         <v>86460</v>
       </c>
-      <c r="E80" s="32">
+      <c r="E80" s="61">
         <v>81720</v>
       </c>
-      <c r="F80" s="54">
+      <c r="F80" s="68">
         <v>4740</v>
       </c>
     </row>
     <row r="81" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="55" t="s">
+      <c r="B81" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C81" s="56">
+      <c r="C81" s="42">
         <v>2012</v>
       </c>
-      <c r="D81" s="57">
+      <c r="D81" s="69">
         <v>26655</v>
       </c>
-      <c r="E81" s="57">
+      <c r="E81" s="69">
         <v>25981</v>
       </c>
-      <c r="F81" s="57">
+      <c r="F81" s="69">
         <v>674</v>
       </c>
     </row>
     <row r="82" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B82" s="21" t="s">
+      <c r="B82" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C82" s="46">
+      <c r="C82" s="28">
         <v>2012</v>
       </c>
-      <c r="D82" s="58">
+      <c r="D82" s="34">
         <v>1779</v>
       </c>
-      <c r="E82" s="58">
+      <c r="E82" s="34">
         <v>1673</v>
       </c>
-      <c r="F82" s="58">
+      <c r="F82" s="34">
         <v>106</v>
       </c>
     </row>
     <row r="83" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="22" t="s">
+      <c r="B83" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C83" s="46">
+      <c r="C83" s="28">
         <v>2012</v>
       </c>
-      <c r="D83" s="58">
+      <c r="D83" s="34">
         <v>41339</v>
       </c>
-      <c r="E83" s="58">
+      <c r="E83" s="34">
         <v>38964</v>
       </c>
-      <c r="F83" s="58">
+      <c r="F83" s="34">
         <v>2375</v>
       </c>
     </row>
     <row r="84" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="22" t="s">
+      <c r="B84" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C84" s="46">
+      <c r="C84" s="28">
         <v>2012</v>
       </c>
-      <c r="D84" s="58">
+      <c r="D84" s="34">
         <v>12870</v>
       </c>
-      <c r="E84" s="58">
+      <c r="E84" s="34">
         <v>11647</v>
       </c>
-      <c r="F84" s="58">
+      <c r="F84" s="34">
         <v>1223</v>
       </c>
     </row>
     <row r="85" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="22" t="s">
+      <c r="B85" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C85" s="46">
+      <c r="C85" s="28">
         <v>2012</v>
       </c>
-      <c r="D85" s="58">
+      <c r="D85" s="34">
         <v>2073</v>
       </c>
-      <c r="E85" s="58">
+      <c r="E85" s="34">
         <v>1875</v>
       </c>
-      <c r="F85" s="58">
+      <c r="F85" s="34">
         <v>198</v>
       </c>
     </row>
     <row r="86" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="22" t="s">
+      <c r="B86" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C86" s="46">
+      <c r="C86" s="28">
         <v>2012</v>
       </c>
-      <c r="D86" s="58">
+      <c r="D86" s="34">
         <v>2700</v>
       </c>
-      <c r="E86" s="58">
+      <c r="E86" s="34">
         <v>2207</v>
       </c>
-      <c r="F86" s="58">
+      <c r="F86" s="34">
         <v>493</v>
       </c>
     </row>
-    <row r="87" spans="2:6" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="24" t="s">
+    <row r="87" spans="2:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B87" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="49">
+      <c r="C87" s="36">
         <v>2012</v>
       </c>
-      <c r="D87" s="59">
+      <c r="D87" s="70">
         <v>87416</v>
       </c>
-      <c r="E87" s="59">
+      <c r="E87" s="70">
         <v>82347</v>
       </c>
-      <c r="F87" s="59">
+      <c r="F87" s="70">
         <v>5069</v>
       </c>
     </row>
     <row r="88" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="21" t="s">
+      <c r="B88" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C88" s="46">
+      <c r="C88" s="28">
         <v>2011</v>
       </c>
-      <c r="D88" s="58">
+      <c r="D88" s="34">
         <v>42076</v>
       </c>
-      <c r="E88" s="58">
+      <c r="E88" s="34">
         <v>41181</v>
       </c>
-      <c r="F88" s="58">
+      <c r="F88" s="34">
         <v>895</v>
       </c>
     </row>
     <row r="89" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="21" t="s">
+      <c r="B89" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C89" s="46">
+      <c r="C89" s="28">
         <v>2011</v>
       </c>
-      <c r="D89" s="58">
+      <c r="D89" s="34">
         <v>1547</v>
       </c>
-      <c r="E89" s="58">
+      <c r="E89" s="34">
         <v>1476</v>
       </c>
-      <c r="F89" s="58">
+      <c r="F89" s="34">
         <v>71</v>
       </c>
     </row>
     <row r="90" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="22" t="s">
+      <c r="B90" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C90" s="46">
+      <c r="C90" s="28">
         <v>2011</v>
       </c>
-      <c r="D90" s="58">
+      <c r="D90" s="34">
         <v>41338</v>
       </c>
-      <c r="E90" s="58">
+      <c r="E90" s="34">
         <v>39147</v>
       </c>
-      <c r="F90" s="58">
+      <c r="F90" s="34">
         <v>2191</v>
       </c>
     </row>
     <row r="91" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="22" t="s">
+      <c r="B91" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C91" s="46">
+      <c r="C91" s="28">
         <v>2011</v>
       </c>
-      <c r="D91" s="58">
+      <c r="D91" s="34">
         <v>12695</v>
       </c>
-      <c r="E91" s="58">
+      <c r="E91" s="34">
         <v>11563</v>
       </c>
-      <c r="F91" s="58">
+      <c r="F91" s="34">
         <v>1132</v>
       </c>
     </row>
     <row r="92" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="22" t="s">
+      <c r="B92" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C92" s="46">
+      <c r="C92" s="28">
         <v>2011</v>
       </c>
-      <c r="D92" s="58">
+      <c r="D92" s="34">
         <v>2267</v>
       </c>
-      <c r="E92" s="58">
+      <c r="E92" s="34">
         <v>1963</v>
       </c>
-      <c r="F92" s="58">
+      <c r="F92" s="34">
         <v>304</v>
       </c>
     </row>
     <row r="93" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="22" t="s">
+      <c r="B93" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C93" s="46">
+      <c r="C93" s="28">
         <v>2011</v>
       </c>
-      <c r="D93" s="58">
+      <c r="D93" s="34">
         <v>2818</v>
       </c>
-      <c r="E93" s="58">
+      <c r="E93" s="34">
         <v>2325</v>
       </c>
-      <c r="F93" s="58">
+      <c r="F93" s="34">
         <v>493</v>
       </c>
     </row>
-    <row r="94" spans="2:6" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B94" s="24" t="s">
+    <row r="94" spans="2:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B94" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C94" s="49">
+      <c r="C94" s="36">
         <v>2011</v>
       </c>
-      <c r="D94" s="59">
+      <c r="D94" s="70">
         <v>102741</v>
       </c>
-      <c r="E94" s="59">
+      <c r="E94" s="70">
         <v>97655</v>
       </c>
-      <c r="F94" s="59">
+      <c r="F94" s="70">
         <v>5086</v>
       </c>
     </row>
     <row r="95" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B95" s="55" t="s">
+      <c r="B95" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C95" s="56">
+      <c r="C95" s="42">
         <v>2010</v>
       </c>
-      <c r="D95" s="57">
+      <c r="D95" s="69">
         <v>24950</v>
       </c>
-      <c r="E95" s="57">
+      <c r="E95" s="69">
         <v>24492</v>
       </c>
-      <c r="F95" s="57">
+      <c r="F95" s="69">
         <v>458</v>
       </c>
     </row>
     <row r="96" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="21" t="s">
+      <c r="B96" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C96" s="46">
+      <c r="C96" s="28">
         <v>2010</v>
       </c>
-      <c r="D96" s="58">
+      <c r="D96" s="34">
         <v>1346</v>
       </c>
-      <c r="E96" s="58">
+      <c r="E96" s="34">
         <v>1252</v>
       </c>
-      <c r="F96" s="58">
+      <c r="F96" s="34">
         <v>94</v>
       </c>
     </row>
     <row r="97" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B97" s="22" t="s">
+      <c r="B97" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C97" s="46">
+      <c r="C97" s="28">
         <v>2010</v>
       </c>
-      <c r="D97" s="58">
+      <c r="D97" s="34">
         <v>41347</v>
       </c>
-      <c r="E97" s="58">
+      <c r="E97" s="34">
         <v>38745</v>
       </c>
-      <c r="F97" s="58">
+      <c r="F97" s="34">
         <v>2602</v>
       </c>
     </row>
     <row r="98" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="22" t="s">
+      <c r="B98" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C98" s="46">
+      <c r="C98" s="28">
         <v>2010</v>
       </c>
-      <c r="D98" s="58">
+      <c r="D98" s="34">
         <v>14462</v>
       </c>
-      <c r="E98" s="58">
+      <c r="E98" s="34">
         <v>12814</v>
       </c>
-      <c r="F98" s="58">
+      <c r="F98" s="34">
         <v>1648</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="22" t="s">
+      <c r="B99" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C99" s="46">
+      <c r="C99" s="28">
         <v>2010</v>
       </c>
-      <c r="D99" s="47">
+      <c r="D99" s="29">
         <v>2153</v>
       </c>
-      <c r="E99" s="47">
+      <c r="E99" s="29">
         <v>1818</v>
       </c>
-      <c r="F99" s="47">
+      <c r="F99" s="29">
         <v>335</v>
       </c>
     </row>
     <row r="100" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="22" t="s">
+      <c r="B100" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C100" s="46">
+      <c r="C100" s="28">
         <v>2010</v>
       </c>
-      <c r="D100" s="47">
+      <c r="D100" s="29">
         <v>3065</v>
       </c>
-      <c r="E100" s="47">
+      <c r="E100" s="29">
         <v>2471</v>
       </c>
-      <c r="F100" s="47">
+      <c r="F100" s="29">
         <v>594</v>
       </c>
     </row>
-    <row r="101" spans="2:6" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="24" t="s">
+    <row r="101" spans="2:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C101" s="49">
+      <c r="C101" s="36">
         <v>2010</v>
       </c>
-      <c r="D101" s="59">
+      <c r="D101" s="70">
         <v>87323</v>
       </c>
-      <c r="E101" s="59">
+      <c r="E101" s="70">
         <v>81592</v>
       </c>
-      <c r="F101" s="59">
+      <c r="F101" s="70">
         <v>5731</v>
       </c>
     </row>
     <row r="102" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="55" t="s">
+      <c r="B102" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C102" s="60">
+      <c r="C102" s="71">
         <v>2005</v>
       </c>
-      <c r="D102" s="61">
+      <c r="D102" s="22">
         <v>20073</v>
       </c>
-      <c r="E102" s="61">
+      <c r="E102" s="22">
         <v>19598</v>
       </c>
-      <c r="F102" s="61">
+      <c r="F102" s="22">
         <v>475</v>
       </c>
     </row>
     <row r="103" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C103" s="60">
+      <c r="C103" s="71">
         <v>2005</v>
       </c>
-      <c r="D103" s="38">
+      <c r="D103" s="22">
         <v>1757</v>
       </c>
-      <c r="E103" s="38">
+      <c r="E103" s="22">
         <v>1655</v>
       </c>
-      <c r="F103" s="38">
+      <c r="F103" s="22">
         <v>102</v>
       </c>
     </row>
     <row r="104" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="22" t="s">
+      <c r="B104" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C104" s="60">
+      <c r="C104" s="71">
         <v>2005</v>
       </c>
-      <c r="D104" s="38">
+      <c r="D104" s="22">
         <v>43181</v>
       </c>
-      <c r="E104" s="38">
+      <c r="E104" s="22">
         <v>40717</v>
       </c>
-      <c r="F104" s="38">
+      <c r="F104" s="22">
         <v>2464</v>
       </c>
     </row>
     <row r="105" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B105" s="22" t="s">
+      <c r="B105" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C105" s="60">
+      <c r="C105" s="71">
         <v>2005</v>
       </c>
-      <c r="D105" s="38">
+      <c r="D105" s="22">
         <v>18693</v>
       </c>
-      <c r="E105" s="38">
+      <c r="E105" s="22">
         <v>16919</v>
       </c>
-      <c r="F105" s="38">
+      <c r="F105" s="22">
         <v>1774</v>
       </c>
     </row>
     <row r="106" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B106" s="22" t="s">
+      <c r="B106" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C106" s="60">
+      <c r="C106" s="71">
         <v>2005</v>
       </c>
-      <c r="D106" s="30">
+      <c r="D106" s="18">
         <v>3384</v>
       </c>
-      <c r="E106" s="30">
+      <c r="E106" s="18">
         <v>2694</v>
       </c>
-      <c r="F106" s="30">
+      <c r="F106" s="18">
         <v>690</v>
       </c>
     </row>
     <row r="107" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B107" s="22" t="s">
+      <c r="B107" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="60">
+      <c r="C107" s="71">
         <v>2005</v>
       </c>
-      <c r="D107" s="30">
+      <c r="D107" s="18">
         <v>4961</v>
       </c>
-      <c r="E107" s="30">
+      <c r="E107" s="18">
         <v>4044</v>
       </c>
-      <c r="F107" s="30">
+      <c r="F107" s="18">
         <v>917</v>
       </c>
     </row>
-    <row r="108" spans="2:6" s="23" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B108" s="24" t="s">
+    <row r="108" spans="2:6" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B108" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C108" s="62">
+      <c r="C108" s="72">
         <v>2005</v>
       </c>
-      <c r="D108" s="42">
+      <c r="D108" s="64">
         <v>92049</v>
       </c>
-      <c r="E108" s="42">
+      <c r="E108" s="64">
         <v>85627</v>
       </c>
-      <c r="F108" s="42">
+      <c r="F108" s="64">
         <v>6422</v>
       </c>
     </row>
     <row r="109" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="63"/>
-      <c r="C109" s="64"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="66"/>
-      <c r="F109" s="66"/>
+      <c r="B109" s="35"/>
+      <c r="C109" s="36"/>
+      <c r="D109" s="37"/>
+      <c r="E109" s="38"/>
+      <c r="F109" s="38"/>
     </row>
     <row r="110" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="67" t="s">
+      <c r="B110" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C110" s="68"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="66"/>
-      <c r="F110" s="66"/>
+      <c r="C110" s="40"/>
+      <c r="D110" s="37"/>
+      <c r="E110" s="38"/>
+      <c r="F110" s="38"/>
     </row>
     <row r="111" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="69" t="s">
+      <c r="B111" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="C111" s="40"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="38"/>
+      <c r="F111" s="38"/>
+    </row>
+    <row r="112" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B112" s="41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C112" s="40"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="38"/>
+      <c r="F112" s="38"/>
+    </row>
+    <row r="113" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="42"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="38"/>
+      <c r="F113" s="38"/>
+    </row>
+    <row r="114" spans="2:6" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B114" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C111" s="68"/>
-      <c r="D111" s="65"/>
-      <c r="E111" s="66"/>
-      <c r="F111" s="66"/>
-    </row>
-    <row r="112" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B112" s="69" t="s">
+      <c r="C114" s="42"/>
+      <c r="D114" s="45"/>
+      <c r="E114" s="46"/>
+      <c r="F114" s="46"/>
+    </row>
+    <row r="115" spans="2:6" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C115" s="31"/>
+    </row>
+    <row r="116" spans="2:6" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B116" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C112" s="68"/>
-      <c r="D112" s="65"/>
-      <c r="E112" s="66"/>
-      <c r="F112" s="66"/>
-    </row>
-    <row r="113" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C113" s="70"/>
-      <c r="D113" s="65"/>
-      <c r="E113" s="66"/>
-      <c r="F113" s="66"/>
-    </row>
-    <row r="114" spans="2:6" s="71" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B114" s="72" t="s">
+      <c r="C116" s="31"/>
+    </row>
+    <row r="117" spans="2:6" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B117" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C114" s="70"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="74"/>
-      <c r="F114" s="74"/>
-    </row>
-    <row r="115" spans="2:6" s="71" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C115" s="51"/>
-    </row>
-    <row r="116" spans="2:6" s="71" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B116" s="71" t="s">
+      <c r="C117" s="31"/>
+    </row>
+    <row r="118" spans="2:6" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B118" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C116" s="51"/>
-    </row>
-    <row r="117" spans="2:6" s="71" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B117" s="71" t="s">
+      <c r="C118" s="31"/>
+    </row>
+    <row r="119" spans="2:6" s="43" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B119" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C117" s="51"/>
-    </row>
-    <row r="118" spans="2:6" s="71" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B118" s="71" t="s">
-        <v>27</v>
-      </c>
-      <c r="C118" s="51"/>
-    </row>
-    <row r="119" spans="2:6" s="71" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B119" s="75" t="s">
-        <v>28</v>
-      </c>
-      <c r="C119" s="51"/>
+      <c r="C119" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>